<commit_message>
Methodology, Risk and cost amendments
Methodology and amendments to cost and risk analysis
</commit_message>
<xml_diff>
--- a/Risk Analysis.xlsx
+++ b/Risk Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Lincoln\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C32896-33D2-4542-8B79-6813227D8358}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ED7833-C282-4842-B507-97BF4C8D5B9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4560" xr2:uid="{9F15B020-5FE2-46B3-968B-90B934D3089B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="63">
   <si>
     <t>Google Cloud</t>
   </si>
@@ -68,12 +68,6 @@
     <t>GDPR - Support for complying with stronger EU data protection laws</t>
   </si>
   <si>
-    <t xml:space="preserve">Independent Security Evaluators (ISE) Audit - Secure Tier 1 feature film’s workload compliance on GCP. </t>
-  </si>
-  <si>
-    <t>Cloud Computing Compliance Controls Catalog (C5) - Information security of cloud services</t>
-  </si>
-  <si>
     <t>ISO - International Organization for Standardization</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>Cloud Security Alliance</t>
   </si>
   <si>
-    <t>PCI DSS - Protecting customers’ card information</t>
-  </si>
-  <si>
     <t>Payment Card Industry Security Standards Council</t>
   </si>
   <si>
@@ -104,9 +95,6 @@
     <t>ISO/IEC 20000-1</t>
   </si>
   <si>
-    <t>ISO - International Organization for Standardization IEC - International Electrotechnical Commission</t>
-  </si>
-  <si>
     <t>CIS Benchmark</t>
   </si>
   <si>
@@ -119,136 +107,348 @@
     <t>Europe</t>
   </si>
   <si>
-    <t>FACT -Federation Against Copyright Theft</t>
-  </si>
-  <si>
     <t>FACT Certification</t>
   </si>
   <si>
-    <t>European Union (EU)</t>
-  </si>
-  <si>
-    <t>European Union (EU)                        United States of America (USA) Switzerland</t>
-  </si>
-  <si>
-    <t>EXCLUDING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azure Batch AI                                                Azure Databricks                                                                Azure Front Door                                            Azure DevOps (formerly VSTS)                                          Azure Firewall                                                             Cognitive Services: Video Indexer                     Storage: Archive                                                                                                                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azure Kubernetes Service (AKS)
-Azure Maps
-Azure Migrate
-Azure Monitor
-Azure Policy
-Azure Resource  Azure Search
-Azure Service Health                          Cloud Shell                                                  Cognitive Services:
-Computer Vision
-Cognitive Services: Content Moderator
-Cognitive Services: Custom Vision
-Cognitive Services: Face
-Cognitive Services: Language Understanding
-Cognitive Services: QnA Maker
-Cognitive Services: Speech Services
-Cognitive Services: Text Analytics
-Cognitive Services: Translator Text
-Cognitive Services: Video Indexer
-Container Instances Container Registry
-Content Delivery Network                                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azure Batch AI                                                        Azure Firewall
-Azure Front Door                                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event Grid                                                                 IoT Central                                                     Machine Learning Services                       Microsoft Genomics                                    Network Watcher                                           Storage: Archive                                                     Time Series Insights                                                Azure Firewall
-Azure Front Door                                                               Azure Database for MySQL
+    <t>✔ (Level 1)</t>
+  </si>
+  <si>
+    <t>Cyber Essentials Plus</t>
+  </si>
+  <si>
+    <t>Data Protection Act 1998</t>
+  </si>
+  <si>
+    <t>CSA STAR - Level 1 - Self-Assessment</t>
+  </si>
+  <si>
+    <t>CSA STAR - Level 2 - Attestation and Certification</t>
+  </si>
+  <si>
+    <t>CSA STAR - Level 3 - Continuous Monitoring</t>
+  </si>
+  <si>
+    <t>Uptime Institute</t>
+  </si>
+  <si>
+    <t>National Cyber Security Centre’s (NCSC) Cloud Security Principles</t>
+  </si>
+  <si>
+    <t>Cloud Security Guidance</t>
+  </si>
+  <si>
+    <t>ISO 31000 - Risk managing</t>
+  </si>
+  <si>
+    <t>PCI DSS (Data Security Standards) - Protecting customers’ card information</t>
+  </si>
+  <si>
+    <t>ISO 14000 family - Environmental management</t>
+  </si>
+  <si>
+    <t>ISO 50001 - Energy management</t>
+  </si>
+  <si>
+    <t>United Kingdom Act of Parliament</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Azure Firewall                                                                                                                                                                   Storage: Archive                                                                                                                                               </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Among others not relevant to Beacon Inc.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Azure Kubernetes Service (AKS)
+Azure Migrate                                                                                                                                                              Cloud Shell                                                                                                                                                               Container Instances                                                                                                                                  Container Registry
+Content Delivery Network                                                                                                                                      IoT Central                                                                                                                                                                    Machine Learning Services                                                                                                               Network Watcher                                                                                                                                    Storage: Archive                                                                                                                                               Azure Firewall                                                                                                                                                       Azure Database for MySQL
 Azure Database for PostgreSQL
 Azure Database Migration Service
-Microsoft Azure Compliance Offerings
-57
-Azure Databricks
+Microsoft Azure Compliance                                                                                                              Azure Databricks
 Azure DDoS Protection
-Azure DevOps (formerly VSTS)                            Azure Active
+Azure DevOps (formerly VSTS)                                                                                                           Azure Active
 Directory Domain Services
 Azure Advisor
 Azure Analysis Services
 Azure Batch AI
 Azure Bot Service
-Azure Container Service                                             Azure Active Directory (Premium P1 + P2)                                                                                                                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azure Batch AI                                                           Azure Databricks                                                             Azure DevOps (formerly VSTS)                                Azure Firewall                                                      Azure Front Door  
-Cognitive Services: Video Indexer          Storage: Archive                                                                                                                                                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azure Batch AI                                                                                                        Azure Firewall                                                    Azure Front Door  
-                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azure Batch AI                                                              Azure Databricks                                                         Azure Firewall
-Azure Front Door                                                      Cognitive Services: Video Indexer            Storage: Archive                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azure Maps                                                                      Azure Service Health                                               BizTalk Services                                                          IoT Central                                                                 Time Series Insights                                                                                                                                                                                                                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azure Database Migration Service             Azure DatabricksAzure DDoS Protection
-Azure DevOps (formerly VSTS)                               Azure Firewall
-Azure Front Door                                                    Azure Maps
-Azure Migrate                                                                Azure Policy                                                               Azure Service Health                                              BizTalk Services                                                         Cognitive Services:
-Computer Vision
-Cognitive Services: Content Moderator
-Cognitive Services: Custom Vision
-Cognitive Services: Face                                        Cognitive Services: Text Analytics
-Cognitive Services: Translator Text
-Cognitive Services: Video Indexer                    Content Delivery Network                                  Data Factory                                                                 IoT Central                                                                   Machine Learning Services                                  Microsoft Genomics                                                  Storage: Archive                                                      Time Series Insights               </t>
-  </si>
-  <si>
-    <t>EU-US Privacy Shield  - A framework for complying with EU Data Protection Directive requirements.</t>
-  </si>
-  <si>
-    <t>✔ (Level 1)</t>
-  </si>
-  <si>
-    <t>Cyber Essentials Plus</t>
-  </si>
-  <si>
-    <t>National Cyber Security Centre (UK)</t>
-  </si>
-  <si>
-    <t>CISPE (Cloud Infrastructure Services Providers in Europe) - helps customers ensure that their cloud infrastructure provider is using appropriate data protection standards to protect their data</t>
-  </si>
-  <si>
-    <t>Data Protection Act 1998</t>
-  </si>
-  <si>
-    <t> United Kingdom Act of Parliament</t>
-  </si>
-  <si>
-    <t>CSA STAR - Level 1 - Self-Assessment</t>
-  </si>
-  <si>
-    <t>CSA STAR - Level 2 - Attestation and Certification</t>
-  </si>
-  <si>
-    <t>CSA STAR - Level 3 - Continuous Monitoring</t>
-  </si>
-  <si>
-    <t>ICREA "International Computer Room Experts Association"</t>
-  </si>
-  <si>
-    <t>Uptime Institute</t>
-  </si>
-  <si>
-    <t>✔ (Tier 3)</t>
-  </si>
-  <si>
-    <t>National Cyber Security Centre’s (NCSC) Cloud Security Principles</t>
-  </si>
-  <si>
-    <t>Cloud Security Guidance</t>
+Azure Container Service                                                                                                                               Azure Active Directory (Premium P1 + P2)                                                                </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Among others not relevant to Beacon Inc.                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                                 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Azure Batch AI                                                                                                                                                                                Azure Firewall
+Azure Front Door                                                                                                                                           </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Among others not relevant to Beacon Inc.    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Azure Batch AI                                                                                                                                                          Azure Databricks                                                                                                                                                      Azure DevOps (formerly VSTS)                                                                                                            Azure Firewall                                                                                                                                                                   Azure Front Door  
+Storage: Archive                                                                                                                                                       </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Among others not relevant to Beacon Inc.   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                         </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Azure Batch AI                                                                                                                                                             Azure Firewall                                                                                                                                                                 Azure Front Door  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Among others not relevant to Beacon Inc.       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">             </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Azure Batch AI                                                                                                                                                      Azure Databricks                                                                                                                                                      Azure Firewall
+Azure Front Door                                                                                                                                         Storage: Archive                                                                                                                                            </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Among others not relevant to Beacon Inc.                 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Azure Service Health                                                                                                                                                  IoT Central                                                                                                                                                                          </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Among others not relevant to Beacon Inc.         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                                                                                                                                                           </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Azure Maps                                                                                                                                                                       Azure Service Health                                                                                                                                                   IoT Central                                                                                                                                                                </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Among others not relevant to Beacon Inc.                    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                                                                                                                                                                                       </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Azure Service Health                                                                                                                                                    IoT Central                                                                                                                                                                          </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Among others not relevant to Beacon Inc.                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                                                                                                                                                                                               </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Azure Database Migration Service                                                                                   Azure DatabricksAzure DDoS Protection
+Azure DevOps (formerly VSTS)                                                          Azure Firewall
+Azure Front Door                                                    
+Azure Migrate                                                                                                                            Azure Service Health                                                                                BizTalk Services                                                                                             Content Delivery Network                                                                Data Factory                                                                                                                   IoT Central                                                                                                             Machine Learning Services                                                                                Storage: Archive                                                                                                </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Among others not relevant to Beacon Inc.            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                  </t>
+    </r>
+  </si>
+  <si>
+    <t>International Organization for Standardization</t>
+  </si>
+  <si>
+    <t>International Organization for Standardization                                 International Electrotechnical Commission</t>
+  </si>
+  <si>
+    <t>European Union                                   United States of America                Switzerland</t>
+  </si>
+  <si>
+    <t>Federation Against Copyright Theft</t>
+  </si>
+  <si>
+    <t>National Cyber Security Centre</t>
+  </si>
+  <si>
+    <t>Excluding</t>
+  </si>
+  <si>
+    <t>Uptime Institute - Tier 3</t>
+  </si>
+  <si>
+    <t>Cloud Infrastructure Services Providers in Europe</t>
+  </si>
+  <si>
+    <t>CISPE - Ensures appropriate data protection standards are being used</t>
+  </si>
+  <si>
+    <t>European Union</t>
+  </si>
+  <si>
+    <t>Organisation</t>
+  </si>
+  <si>
+    <t>Standard/Certification/Regulation</t>
+  </si>
+  <si>
+    <t>EU-US Privacy Shield  - Framework for complying with EU Data Protection Directive requirements.</t>
   </si>
 </sst>
 </file>
@@ -259,13 +459,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,18 +500,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -356,7 +552,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -413,229 +609,102 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="7" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
-    <cellStyle name="Accent2" xfId="6" builtinId="33"/>
-    <cellStyle name="Accent5" xfId="7" builtinId="45"/>
-    <cellStyle name="Accent6" xfId="8" builtinId="49"/>
-    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
-    <cellStyle name="Input" xfId="2" builtinId="20"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+  <cellStyles count="8">
+    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="5" builtinId="33"/>
+    <cellStyle name="Accent5" xfId="6" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="7" builtinId="49"/>
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -953,34 +1022,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE20D6AA-BB18-4054-BDA7-20DF0AA9818A}">
-  <dimension ref="A1:U440"/>
+  <dimension ref="A1:M437"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="36" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="42" customWidth="1"/>
-    <col min="4" max="4" width="14" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="46" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="14" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="26" t="s">
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>2</v>
@@ -989,417 +1062,513 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="7"/>
+    <row r="2" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="59.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="106.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="1">
+        <v>16</v>
+      </c>
+      <c r="J8" s="2">
+        <v>20</v>
+      </c>
+      <c r="K8" s="3">
+        <v>17</v>
+      </c>
+      <c r="L8" s="24">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="G17" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="F20" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="F21" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="M24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:21" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="D25" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:21" ht="361.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:21" ht="392.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="7" spans="1:21" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="24"/>
-    </row>
-    <row r="8" spans="1:21" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="40"/>
-      <c r="F13" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="S13" s="3">
-        <v>15</v>
-      </c>
-      <c r="T13" s="2">
-        <v>19</v>
-      </c>
-      <c r="U13" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="405" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="41"/>
-      <c r="F23" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" s="45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
@@ -1407,7 +1576,7 @@
       <c r="F30"/>
       <c r="G30"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
@@ -1415,7 +1584,7 @@
       <c r="F31"/>
       <c r="G31"/>
     </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
@@ -4663,30 +4832,6 @@
       <c r="F437"/>
       <c r="G437"/>
     </row>
-    <row r="438" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B438"/>
-      <c r="C438"/>
-      <c r="D438"/>
-      <c r="E438"/>
-      <c r="F438"/>
-      <c r="G438"/>
-    </row>
-    <row r="439" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B439"/>
-      <c r="C439"/>
-      <c r="D439"/>
-      <c r="E439"/>
-      <c r="F439"/>
-      <c r="G439"/>
-    </row>
-    <row r="440" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B440"/>
-      <c r="C440"/>
-      <c r="D440"/>
-      <c r="E440"/>
-      <c r="F440"/>
-      <c r="G440"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>